<commit_message>
Update misure - needs review
</commit_message>
<xml_diff>
--- a/DocMisureProg.xlsx
+++ b/DocMisureProg.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="159">
   <si>
     <t>Glossario</t>
   </si>
@@ -438,33 +438,12 @@
     <t>Notifica</t>
   </si>
   <si>
-    <t>Eventi</t>
-  </si>
-  <si>
-    <t>Data element</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Dati</t>
-  </si>
-  <si>
     <t>Rank</t>
   </si>
   <si>
     <t>Note</t>
   </si>
   <si>
-    <t>D.E. = Dati evento, Persone collegate, Documenti collegati</t>
-  </si>
-  <si>
-    <t>D.E. = Dati evento</t>
-  </si>
-  <si>
-    <t>D.E. = Urgenza, Timestamp, Inizio/Fine, Desc, Notifica</t>
-  </si>
-  <si>
     <t>Transizioni</t>
   </si>
   <si>
@@ -477,35 +456,56 @@
     <t>1 * 3 = 3</t>
   </si>
   <si>
-    <t>1 * 7 = 7</t>
+    <t>Function Points CALENDARIO</t>
+  </si>
+  <si>
+    <t>VAF = 0.65 + 0.12 = 0.77</t>
+  </si>
+  <si>
+    <t>Total FC</t>
+  </si>
+  <si>
+    <t>28/03/2019</t>
+  </si>
+  <si>
+    <t>Data Elements = Dati evento, Persone, Documenti --- FTR = Eventi</t>
+  </si>
+  <si>
+    <t>D.E. = Dati evento, Persone, Documenti --- FTR = Eventi</t>
+  </si>
+  <si>
+    <t>D.E. = Dati evento --- FTR = Eventi</t>
+  </si>
+  <si>
+    <t>EI, ILF</t>
+  </si>
+  <si>
+    <t>EQ, ILF</t>
+  </si>
+  <si>
+    <t>EO, ILF</t>
   </si>
   <si>
     <t>0 * 5 = 0</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Function Points CALENDARIO</t>
-  </si>
-  <si>
-    <t>VAF = 0.65 + 0.12 = 0.77</t>
-  </si>
-  <si>
-    <t>Total FC</t>
-  </si>
-  <si>
-    <t>Function Point = 23 * 0.77 = 17.71</t>
-  </si>
-  <si>
-    <t>28/03/2019</t>
+    <t>5 * 7 = 35</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>5 perché appare in ogni funzione? o 1 perché ci sono solo gli "Eventi"??</t>
+  </si>
+  <si>
+    <t>Function Point = 48 * 0.77 = 39.27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +536,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -646,9 +653,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,6 +719,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1219,8 +1224,8 @@
   </sheetPr>
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+    <sheetView tabSelected="1" topLeftCell="I10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,18 +1235,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="42" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="41" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1250,13 +1255,13 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
-      <c r="Q1" s="25" t="s">
-        <v>154</v>
+      <c r="Q1" s="24" t="s">
+        <v>144</v>
       </c>
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
       <c r="T1" s="11" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="U1" s="11"/>
       <c r="V1" s="1"/>
@@ -1271,11 +1276,11 @@
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1288,24 +1293,18 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
-      <c r="Q2" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="27" t="s">
+      <c r="Q2" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="R2" s="37"/>
+      <c r="S2" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="25" t="s">
         <v>139</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="W2" s="26" t="s">
-        <v>143</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -1338,24 +1337,18 @@
       <c r="N3" s="3"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="32" t="s">
+      <c r="Q3" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="R3" s="32"/>
+      <c r="R3" s="31"/>
       <c r="S3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="T3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>144</v>
+      <c r="U3" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -1378,36 +1371,30 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="R4" s="32"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="T4" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>144</v>
+      <c r="U4" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -1430,36 +1417,30 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="R5" s="32"/>
+      <c r="R5" s="31"/>
       <c r="S5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V5" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="T5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>145</v>
+      <c r="U5" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -1482,36 +1463,30 @@
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="32"/>
+      <c r="R6" s="31"/>
       <c r="S6" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="T6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V6" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="T6" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>144</v>
+      <c r="U6" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -1526,36 +1501,30 @@
       <c r="D7" s="3"/>
       <c r="E7" s="11"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="32" t="s">
+      <c r="Q7" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="R7" s="32"/>
+      <c r="R7" s="31"/>
       <c r="S7" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V7" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="T7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="W7" s="1" t="s">
-        <v>145</v>
+      <c r="U7" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -1567,38 +1536,30 @@
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="11"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="R8" s="35"/>
-      <c r="S8" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="T8" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="U8" s="28" t="s">
-        <v>27</v>
-      </c>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="26"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="27"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
@@ -1622,37 +1583,25 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="32" t="s">
-        <v>138</v>
-      </c>
-      <c r="R9" s="32"/>
-      <c r="S9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="V9" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>146</v>
-      </c>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -1674,13 +1623,13 @@
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
@@ -1712,28 +1661,28 @@
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="36" t="s">
+      <c r="Q11" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="33" t="s">
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="U11" s="33"/>
-      <c r="V11" s="33"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
@@ -1755,31 +1704,31 @@
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="23" t="s">
+      <c r="Q12" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="23" t="s">
+      <c r="R12" s="22" t="s">
         <v>16</v>
       </c>
       <c r="S12" s="11"/>
-      <c r="T12" s="37" t="s">
+      <c r="T12" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="U12" s="37"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="37"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
       <c r="X12" s="21" t="s">
         <v>108</v>
       </c>
@@ -1793,34 +1742,34 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="U13" s="32" t="s">
+      <c r="U13" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="30">
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="29">
         <v>0</v>
       </c>
       <c r="Y13" s="1"/>
@@ -1831,39 +1780,39 @@
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="41"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="23" t="s">
+      <c r="Q14" s="22" t="s">
         <v>35</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="S14" s="11"/>
       <c r="T14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="U14" s="32" t="s">
+      <c r="U14" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="30">
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="29">
         <v>0</v>
       </c>
       <c r="Y14" s="1"/>
@@ -1885,34 +1834,34 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="42" t="s">
+      <c r="G15" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="23" t="s">
+      <c r="Q15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="R15" s="10" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="S15" s="11"/>
       <c r="T15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="U15" s="32" t="s">
+      <c r="U15" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
-      <c r="X15" s="30">
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="29">
         <v>0</v>
       </c>
       <c r="Y15" s="1"/>
@@ -1934,34 +1883,36 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
+      <c r="O16" s="46" t="s">
+        <v>157</v>
+      </c>
       <c r="P16" s="3"/>
-      <c r="Q16" s="23" t="s">
+      <c r="Q16" s="22" t="s">
         <v>37</v>
       </c>
       <c r="R16" s="10" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="S16" s="11"/>
       <c r="T16" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="U16" s="32" t="s">
+      <c r="U16" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="30">
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="29">
         <v>1</v>
       </c>
       <c r="Y16" s="1"/>
@@ -1983,34 +1934,34 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="23" t="s">
+      <c r="Q17" s="22" t="s">
         <v>38</v>
       </c>
       <c r="R17" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="S17" s="11"/>
       <c r="T17" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="U17" s="32" t="s">
+      <c r="U17" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="30">
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="29">
         <v>1</v>
       </c>
       <c r="Y17" s="1"/>
@@ -2042,22 +1993,22 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="23" t="s">
+      <c r="Q18" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="R18" s="10" t="s">
         <v>156</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>153</v>
       </c>
       <c r="S18" s="11"/>
       <c r="T18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="U18" s="32" t="s">
+      <c r="U18" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="30">
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="29">
         <v>0</v>
       </c>
       <c r="Y18" s="1"/>
@@ -2087,12 +2038,12 @@
       <c r="T19" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="U19" s="32" t="s">
+      <c r="U19" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="V19" s="32"/>
-      <c r="W19" s="32"/>
-      <c r="X19" s="30">
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="29">
         <v>4</v>
       </c>
       <c r="Y19" s="1"/>
@@ -2100,21 +2051,21 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="32" t="s">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2126,12 +2077,12 @@
       <c r="T20" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="U20" s="32" t="s">
+      <c r="U20" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="30">
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="29">
         <v>0</v>
       </c>
       <c r="Y20" s="1"/>
@@ -2140,11 +2091,11 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
       <c r="E21" s="14"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -2163,12 +2114,12 @@
       <c r="T21" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="U21" s="32" t="s">
+      <c r="U21" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="30">
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="29">
         <v>0</v>
       </c>
       <c r="Y21" s="1"/>
@@ -2204,12 +2155,12 @@
       <c r="T22" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="32" t="s">
+      <c r="U22" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="30">
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="29">
         <v>1</v>
       </c>
       <c r="Y22" s="1"/>
@@ -2243,12 +2194,12 @@
       <c r="T23" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="U23" s="32" t="s">
+      <c r="U23" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="30">
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="29">
         <v>1</v>
       </c>
       <c r="Y23" s="1"/>
@@ -2282,12 +2233,12 @@
       <c r="T24" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="U24" s="32" t="s">
+      <c r="U24" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="30">
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="29">
         <v>1</v>
       </c>
       <c r="Y24" s="1"/>
@@ -2321,12 +2272,12 @@
       <c r="T25" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="U25" s="32" t="s">
+      <c r="U25" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="V25" s="32"/>
-      <c r="W25" s="32"/>
-      <c r="X25" s="30">
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="29">
         <v>0</v>
       </c>
       <c r="Y25" s="1"/>
@@ -2360,12 +2311,12 @@
       <c r="T26" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="U26" s="32" t="s">
+      <c r="U26" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="V26" s="32"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="30">
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="29">
         <v>3</v>
       </c>
       <c r="Y26" s="1"/>
@@ -2399,24 +2350,24 @@
       <c r="T27" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="U27" s="30">
+      <c r="U27" s="29">
         <f>SUM(X13:X26)</f>
         <v>12</v>
       </c>
-      <c r="V27" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="W27" s="34"/>
-      <c r="X27" s="34"/>
+      <c r="V27" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="W27" s="33"/>
+      <c r="X27" s="33"/>
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="46"/>
+      <c r="D28" s="45"/>
       <c r="E28" s="15"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2442,12 +2393,12 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="R29" s="31"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
+      <c r="Q29" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="R29" s="30"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="30"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
@@ -2458,44 +2409,44 @@
       <c r="AB29" s="1"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="32" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="M30" s="36" t="s">
+      <c r="M30" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="N30" s="36"/>
+      <c r="N30" s="35"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="41" t="s">
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
       <c r="M31" s="17" t="s">
         <v>108</v>
       </c>
@@ -2509,20 +2460,20 @@
       <c r="A32" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32" t="s">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
       <c r="M32" s="17" t="s">
         <v>57</v>
       </c>
@@ -2536,20 +2487,20 @@
       <c r="A33" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
       <c r="M33" s="17" t="s">
         <v>28</v>
       </c>
@@ -2563,20 +2514,20 @@
       <c r="A34" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
       <c r="M34" s="17" t="s">
         <v>58</v>
       </c>
@@ -2590,20 +2541,20 @@
       <c r="A35" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32" t="s">
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
       <c r="M35" s="17" t="s">
         <v>43</v>
       </c>
@@ -2617,20 +2568,20 @@
       <c r="A36" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32" t="s">
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
       <c r="M36" s="17" t="s">
         <v>44</v>
       </c>
@@ -2644,20 +2595,20 @@
       <c r="A37" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32" t="s">
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
       <c r="M37" s="17" t="s">
         <v>45</v>
       </c>
@@ -2671,20 +2622,20 @@
       <c r="A38" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32" t="s">
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="31"/>
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
     </row>
@@ -2692,20 +2643,20 @@
       <c r="A39" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32" t="s">
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="31"/>
+      <c r="K39" s="31"/>
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
     </row>
@@ -2713,20 +2664,20 @@
       <c r="A40" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32" t="s">
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
+      <c r="K40" s="31"/>
       <c r="O40" s="20"/>
       <c r="P40" s="20"/>
     </row>
@@ -2734,20 +2685,20 @@
       <c r="A41" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32" t="s">
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
       <c r="O41" s="20"/>
       <c r="P41" s="20"/>
     </row>
@@ -2755,20 +2706,20 @@
       <c r="A42" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32" t="s">
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+      <c r="J42" s="31"/>
+      <c r="K42" s="31"/>
       <c r="O42" s="20"/>
       <c r="P42" s="20"/>
     </row>
@@ -2776,20 +2727,20 @@
       <c r="A43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32" t="s">
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+      <c r="J43" s="31"/>
+      <c r="K43" s="31"/>
       <c r="O43" s="20"/>
       <c r="P43" s="20"/>
     </row>
@@ -2797,20 +2748,20 @@
       <c r="A44" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32" t="s">
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
       <c r="O44" s="20"/>
       <c r="P44" s="20"/>
     </row>
@@ -2818,20 +2769,20 @@
       <c r="A45" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32" t="s">
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31"/>
+      <c r="K45" s="31"/>
       <c r="O45" s="20"/>
       <c r="P45" s="20"/>
     </row>
@@ -2872,93 +2823,93 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="B49" s="36"/>
+      <c r="B49" s="35"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="36"/>
+      <c r="B53" s="35"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="40" t="s">
+      <c r="A54" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="40"/>
-      <c r="C54" s="39" t="s">
+      <c r="B54" s="39"/>
+      <c r="C54" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="40" t="s">
+      <c r="A55" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="40"/>
-      <c r="C55" s="39" t="s">
+      <c r="B55" s="39"/>
+      <c r="C55" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="40" t="s">
+      <c r="A56" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="39" t="s">
+      <c r="B56" s="39"/>
+      <c r="C56" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="40" t="s">
+      <c r="A57" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="39" t="s">
+      <c r="B57" s="39"/>
+      <c r="C57" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="40" t="s">
+      <c r="A58" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="39" t="s">
+      <c r="B58" s="39"/>
+      <c r="C58" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="39"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="38"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="40"/>
-      <c r="C59" s="39" t="s">
+      <c r="B59" s="39"/>
+      <c r="C59" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="D59" s="39"/>
-      <c r="E59" s="39"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="98">

</xml_diff>

<commit_message>
Meeting 03/04/19 (vedi verbale)
</commit_message>
<xml_diff>
--- a/DocMisureProg.xlsx
+++ b/DocMisureProg.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="152">
   <si>
     <t>Glossario</t>
   </si>
@@ -447,27 +447,9 @@
     <t>Transizioni</t>
   </si>
   <si>
-    <t>3 * 3 = 9</t>
-  </si>
-  <si>
-    <t>1 * 4 = 4</t>
-  </si>
-  <si>
-    <t>1 * 3 = 3</t>
-  </si>
-  <si>
-    <t>Function Points CALENDARIO</t>
-  </si>
-  <si>
-    <t>VAF = 0.65 + 0.12 = 0.77</t>
-  </si>
-  <si>
     <t>Total FC</t>
   </si>
   <si>
-    <t>28/03/2019</t>
-  </si>
-  <si>
     <t>Data Elements = Dati evento, Persone, Documenti --- FTR = Eventi</t>
   </si>
   <si>
@@ -486,19 +468,16 @@
     <t>EO, ILF</t>
   </si>
   <si>
-    <t>0 * 5 = 0</t>
-  </si>
-  <si>
-    <t>5 * 7 = 35</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>5 perché appare in ogni funzione? o 1 perché ci sono solo gli "Eventi"??</t>
-  </si>
-  <si>
-    <t>Function Point = 48 * 0.77 = 39.27</t>
+    <t xml:space="preserve">VAF = 0.65 + 0.12 = </t>
+  </si>
+  <si>
+    <t>Function Points =</t>
+  </si>
+  <si>
+    <t>03/04/2019</t>
+  </si>
+  <si>
+    <t>Calcolo Function Points CALENDARIO</t>
   </si>
 </sst>
 </file>
@@ -604,7 +583,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -656,70 +635,85 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1224,29 +1218,30 @@
   </sheetPr>
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q30"/>
+    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -1254,16 +1249,16 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="U1" s="11"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="11" t="s">
+        <v>150</v>
+      </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -1276,11 +1271,11 @@
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -1292,24 +1287,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="R2" s="37"/>
-      <c r="S2" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="T2" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="U2" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
+      <c r="P2" s="49"/>
       <c r="AB2" s="1"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
@@ -1336,19 +1314,19 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="R3" s="31"/>
-      <c r="S3" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="T3" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>148</v>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="R3" s="42"/>
+      <c r="S3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="T3" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="U3" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -1371,30 +1349,30 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="R4" s="31"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="R4" s="30"/>
       <c r="S4" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="T4" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="T4" s="25" t="s">
         <v>16</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
@@ -1417,30 +1395,30 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="R5" s="31"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" s="30"/>
       <c r="S5" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="T5" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="T5" s="25" t="s">
         <v>16</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
@@ -1463,30 +1441,30 @@
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="R6" s="31"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="R6" s="30"/>
       <c r="S6" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="T6" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="T6" s="25" t="s">
         <v>16</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -1501,30 +1479,30 @@
       <c r="D7" s="3"/>
       <c r="E7" s="11"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="41" t="s">
+      <c r="G7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="R7" s="31"/>
+      <c r="P7" s="49"/>
+      <c r="Q7" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="R7" s="30"/>
       <c r="S7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="T7" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="T7" s="25" t="s">
         <v>16</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -1536,32 +1514,38 @@
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="11"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="R8" s="30"/>
+      <c r="S8" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="T8" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
@@ -1583,30 +1567,27 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="31"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
-      <c r="V9" s="28"/>
+      <c r="V9" s="25"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -1623,16 +1604,16 @@
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="P10" s="49"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
@@ -1642,9 +1623,6 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
@@ -1661,33 +1639,31 @@
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="41" t="s">
+      <c r="G11" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="35" t="s">
+      <c r="P11" s="49"/>
+      <c r="Q11" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="32" t="s">
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="U11" s="32"/>
-      <c r="V11" s="32"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
@@ -1704,18 +1680,18 @@
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="41" t="s">
+      <c r="G12" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="49"/>
       <c r="Q12" s="22" t="s">
         <v>39</v>
       </c>
@@ -1723,17 +1699,15 @@
         <v>16</v>
       </c>
       <c r="S12" s="11"/>
-      <c r="T12" s="36" t="s">
+      <c r="T12" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
+      <c r="U12" s="33"/>
+      <c r="V12" s="33"/>
+      <c r="W12" s="33"/>
       <c r="X12" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -1742,82 +1716,78 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
+      <c r="P13" s="49"/>
       <c r="Q13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="10" t="s">
-        <v>141</v>
+      <c r="R13" s="43" t="s">
+        <v>43</v>
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="U13" s="31" t="s">
+      <c r="U13" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="29">
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="26">
         <v>0</v>
       </c>
       <c r="Y13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
+      <c r="P14" s="49"/>
       <c r="Q14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="R14" s="10" t="s">
-        <v>142</v>
+      <c r="R14" s="43" t="s">
+        <v>28</v>
       </c>
       <c r="S14" s="11"/>
       <c r="T14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="U14" s="31" t="s">
+      <c r="U14" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="29">
+      <c r="V14" s="30"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="26">
         <v>0</v>
       </c>
       <c r="Y14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
@@ -1834,34 +1804,34 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
+      <c r="P15" s="49"/>
       <c r="Q15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="R15" s="10" t="s">
-        <v>143</v>
+      <c r="R15" s="43" t="s">
+        <v>28</v>
       </c>
       <c r="S15" s="11"/>
       <c r="T15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="U15" s="31" t="s">
+      <c r="U15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="29">
+      <c r="V15" s="30"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="26">
         <v>0</v>
       </c>
       <c r="Y15" s="1"/>
@@ -1883,36 +1853,34 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="46" t="s">
-        <v>157</v>
-      </c>
-      <c r="P16" s="3"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="49"/>
       <c r="Q16" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="R16" s="10" t="s">
-        <v>155</v>
+      <c r="R16" s="43" t="s">
+        <v>45</v>
       </c>
       <c r="S16" s="11"/>
       <c r="T16" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="U16" s="31" t="s">
+      <c r="U16" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="29">
+      <c r="V16" s="30"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="26">
         <v>1</v>
       </c>
       <c r="Y16" s="1"/>
@@ -1934,34 +1902,34 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
+      <c r="P17" s="49"/>
       <c r="Q17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="R17" s="10" t="s">
-        <v>154</v>
+      <c r="R17" s="43" t="s">
+        <v>57</v>
       </c>
       <c r="S17" s="11"/>
       <c r="T17" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="U17" s="31" t="s">
+      <c r="U17" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="29">
+      <c r="V17" s="30"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="26">
         <v>1</v>
       </c>
       <c r="Y17" s="1"/>
@@ -1992,23 +1960,24 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
+      <c r="P18" s="49"/>
       <c r="Q18" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>156</v>
+        <v>141</v>
+      </c>
+      <c r="R18" s="43">
+        <f xml:space="preserve"> SUM(3*R13,4*R14,3*R15,7*R16,5*R17)</f>
+        <v>51</v>
       </c>
       <c r="S18" s="11"/>
       <c r="T18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="U18" s="31" t="s">
+      <c r="U18" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="29">
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="26">
         <v>0</v>
       </c>
       <c r="Y18" s="1"/>
@@ -2031,19 +2000,19 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
+      <c r="P19" s="49"/>
       <c r="Q19" s="11"/>
       <c r="R19" s="11"/>
       <c r="S19" s="11"/>
       <c r="T19" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="U19" s="31" t="s">
+      <c r="U19" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="29">
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="26">
         <v>4</v>
       </c>
       <c r="Y19" s="1"/>
@@ -2051,38 +2020,38 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="31" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="30"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
+      <c r="P20" s="49"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
       <c r="S20" s="11"/>
       <c r="T20" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="U20" s="31" t="s">
+      <c r="U20" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="29">
+      <c r="V20" s="30"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="26">
         <v>0</v>
       </c>
       <c r="Y20" s="1"/>
@@ -2091,11 +2060,11 @@
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="45"/>
-      <c r="D21" s="45"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="14"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -2107,19 +2076,19 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
+      <c r="P21" s="49"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
       <c r="S21" s="11"/>
       <c r="T21" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="U21" s="31" t="s">
+      <c r="U21" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="29">
+      <c r="V21" s="30"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="26">
         <v>0</v>
       </c>
       <c r="Y21" s="1"/>
@@ -2148,19 +2117,19 @@
       <c r="I22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
+      <c r="P22" s="49"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
       <c r="T22" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="U22" s="31" t="s">
+      <c r="U22" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="29">
+      <c r="V22" s="30"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="26">
         <v>1</v>
       </c>
       <c r="Y22" s="1"/>
@@ -2187,19 +2156,19 @@
       <c r="I23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
+      <c r="P23" s="49"/>
       <c r="Q23" s="11"/>
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
       <c r="T23" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="U23" s="31" t="s">
+      <c r="U23" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="29">
+      <c r="V23" s="30"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="26">
         <v>1</v>
       </c>
       <c r="Y23" s="1"/>
@@ -2226,19 +2195,19 @@
       <c r="I24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+      <c r="P24" s="49"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="11"/>
       <c r="S24" s="11"/>
       <c r="T24" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="U24" s="31" t="s">
+      <c r="U24" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="29">
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="26">
         <v>1</v>
       </c>
       <c r="Y24" s="1"/>
@@ -2265,19 +2234,19 @@
       <c r="I25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
+      <c r="P25" s="49"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="11"/>
       <c r="S25" s="11"/>
       <c r="T25" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="U25" s="31" t="s">
+      <c r="U25" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="29">
+      <c r="V25" s="30"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="26">
         <v>0</v>
       </c>
       <c r="Y25" s="1"/>
@@ -2304,19 +2273,19 @@
       <c r="I26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
+      <c r="P26" s="49"/>
       <c r="Q26" s="11"/>
       <c r="R26" s="11"/>
       <c r="S26" s="11"/>
       <c r="T26" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="U26" s="31" t="s">
+      <c r="U26" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="29">
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="26">
         <v>3</v>
       </c>
       <c r="Y26" s="1"/>
@@ -2343,31 +2312,34 @@
       <c r="I27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
+      <c r="P27" s="49"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
       <c r="S27" s="11"/>
       <c r="T27" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="U27" s="29">
-        <f>SUM(X13:X26)</f>
+      <c r="U27" s="25">
+        <f>SUM(X12:X26)</f>
         <v>12</v>
       </c>
-      <c r="V27" s="33" t="s">
-        <v>145</v>
-      </c>
-      <c r="W27" s="33"/>
-      <c r="X27" s="33"/>
+      <c r="V27" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="W27" s="46"/>
+      <c r="X27" s="48">
+        <f xml:space="preserve"> 0.65 + (U27/100)</f>
+        <v>0.77</v>
+      </c>
       <c r="AB27" s="1"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="45"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="15"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2375,7 +2347,7 @@
       <c r="I28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
+      <c r="P28" s="49"/>
       <c r="V28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
@@ -2392,13 +2364,8 @@
       <c r="I29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
+      <c r="P29" s="49"/>
+      <c r="T29" s="44"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
@@ -2409,44 +2376,52 @@
       <c r="AB29" s="1"/>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="31" t="s">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="M30" s="35" t="s">
+      <c r="M30" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="N30" s="35"/>
+      <c r="N30" s="29"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
+      <c r="P30" s="49"/>
+      <c r="R30" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="S30" s="45"/>
+      <c r="T30" s="47">
+        <f xml:space="preserve"> R18*X27</f>
+        <v>39.270000000000003</v>
+      </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="40" t="s">
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
       <c r="M31" s="17" t="s">
         <v>108</v>
       </c>
@@ -2454,26 +2429,26 @@
         <v>59</v>
       </c>
       <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
+      <c r="P31" s="49"/>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31" t="s">
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
       <c r="M32" s="17" t="s">
         <v>57</v>
       </c>
@@ -2481,26 +2456,26 @@
         <v>60</v>
       </c>
       <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
+      <c r="P32" s="51"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31" t="s">
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="30"/>
+      <c r="K33" s="30"/>
       <c r="M33" s="17" t="s">
         <v>28</v>
       </c>
@@ -2508,26 +2483,26 @@
         <v>65</v>
       </c>
       <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
+      <c r="P33" s="51"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
       <c r="M34" s="17" t="s">
         <v>58</v>
       </c>
@@ -2535,26 +2510,26 @@
         <v>61</v>
       </c>
       <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
+      <c r="P34" s="51"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31" t="s">
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
       <c r="M35" s="17" t="s">
         <v>43</v>
       </c>
@@ -2562,26 +2537,26 @@
         <v>62</v>
       </c>
       <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
+      <c r="P35" s="51"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31" t="s">
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
       <c r="M36" s="17" t="s">
         <v>44</v>
       </c>
@@ -2589,26 +2564,26 @@
         <v>63</v>
       </c>
       <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
+      <c r="P36" s="51"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31" t="s">
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
       <c r="M37" s="17" t="s">
         <v>45</v>
       </c>
@@ -2616,175 +2591,175 @@
         <v>64</v>
       </c>
       <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
+      <c r="P37" s="51"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31" t="s">
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="31"/>
-      <c r="K38" s="31"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
       <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
+      <c r="P38" s="51"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31" t="s">
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
-      <c r="K39" s="31"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
       <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
+      <c r="P39" s="51"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31" t="s">
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
       <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
+      <c r="P40" s="51"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31" t="s">
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="30"/>
       <c r="O41" s="20"/>
-      <c r="P41" s="20"/>
+      <c r="P41" s="51"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31" t="s">
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
       <c r="O42" s="20"/>
-      <c r="P42" s="20"/>
+      <c r="P42" s="51"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31" t="s">
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="31"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="30"/>
       <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
+      <c r="P43" s="51"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31" t="s">
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="31"/>
-      <c r="I44" s="31"/>
-      <c r="J44" s="31"/>
-      <c r="K44" s="31"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="30"/>
+      <c r="K44" s="30"/>
       <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
+      <c r="P44" s="51"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31" t="s">
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
       <c r="O45" s="20"/>
-      <c r="P45" s="20"/>
+      <c r="P45" s="51"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
@@ -2799,7 +2774,7 @@
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
+      <c r="P46" s="49"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
@@ -2812,7 +2787,7 @@
       <c r="H47" s="3"/>
       <c r="I47" s="3"/>
       <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
+      <c r="P47" s="49"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C48" s="1"/>
@@ -2821,98 +2796,196 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
+      <c r="P48" s="52"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B49" s="35"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="30" t="s">
+      <c r="P49" s="52"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="7"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="P50" s="52"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P51" s="52"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P52" s="52"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B53" s="35"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="39" t="s">
+      <c r="B53" s="29"/>
+      <c r="P53" s="52"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="38" t="s">
+      <c r="B54" s="40"/>
+      <c r="C54" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
+      <c r="P54" s="52"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B55" s="39"/>
-      <c r="C55" s="38" t="s">
+      <c r="B55" s="40"/>
+      <c r="C55" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
+      <c r="P55" s="52"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="B56" s="39"/>
-      <c r="C56" s="38" t="s">
+      <c r="B56" s="40"/>
+      <c r="C56" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="P56" s="52"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="38" t="s">
+      <c r="B57" s="40"/>
+      <c r="C57" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="39" t="s">
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
+      <c r="P57" s="52"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="38" t="s">
+      <c r="B58" s="40"/>
+      <c r="C58" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="38"/>
-      <c r="E58" s="38"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="P58" s="52"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="38" t="s">
+      <c r="B59" s="40"/>
+      <c r="C59" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="P59" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="98">
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="U25:W25"/>
+    <mergeCell ref="U26:W26"/>
+    <mergeCell ref="T11:V11"/>
+    <mergeCell ref="U19:W19"/>
+    <mergeCell ref="U20:W20"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="U23:W23"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="U17:W17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="T12:W12"/>
+    <mergeCell ref="U13:W13"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="E35:K35"/>
+    <mergeCell ref="E34:K34"/>
+    <mergeCell ref="E33:K33"/>
+    <mergeCell ref="E32:K32"/>
+    <mergeCell ref="E31:K31"/>
+    <mergeCell ref="E45:K45"/>
+    <mergeCell ref="E44:K44"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="E42:K42"/>
+    <mergeCell ref="E41:K41"/>
+    <mergeCell ref="E40:K40"/>
+    <mergeCell ref="E39:K39"/>
+    <mergeCell ref="E38:K38"/>
+    <mergeCell ref="E37:K37"/>
+    <mergeCell ref="E36:K36"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="G11:M11"/>
+    <mergeCell ref="G9:M9"/>
+    <mergeCell ref="G14:M14"/>
+    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="G16:M16"/>
+    <mergeCell ref="G15:M15"/>
+    <mergeCell ref="G13:M13"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="G17:M17"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="B44:D44"/>
     <mergeCell ref="B45:D45"/>
@@ -2929,88 +3002,6 @@
     <mergeCell ref="G7:M7"/>
     <mergeCell ref="G6:M6"/>
     <mergeCell ref="G5:M5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="G17:M17"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="G16:M16"/>
-    <mergeCell ref="G15:M15"/>
-    <mergeCell ref="G13:M13"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="G11:M11"/>
-    <mergeCell ref="G9:M9"/>
-    <mergeCell ref="G14:M14"/>
-    <mergeCell ref="G10:M10"/>
-    <mergeCell ref="E40:K40"/>
-    <mergeCell ref="E39:K39"/>
-    <mergeCell ref="E38:K38"/>
-    <mergeCell ref="E37:K37"/>
-    <mergeCell ref="E36:K36"/>
-    <mergeCell ref="E45:K45"/>
-    <mergeCell ref="E44:K44"/>
-    <mergeCell ref="E43:K43"/>
-    <mergeCell ref="E42:K42"/>
-    <mergeCell ref="E41:K41"/>
-    <mergeCell ref="E35:K35"/>
-    <mergeCell ref="E34:K34"/>
-    <mergeCell ref="E33:K33"/>
-    <mergeCell ref="E32:K32"/>
-    <mergeCell ref="E31:K31"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="U13:W13"/>
-    <mergeCell ref="Q29:T29"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="U25:W25"/>
-    <mergeCell ref="U26:W26"/>
-    <mergeCell ref="T11:V11"/>
-    <mergeCell ref="V27:X27"/>
-    <mergeCell ref="U19:W19"/>
-    <mergeCell ref="U20:W20"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="U23:W23"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="U17:W17"/>
-    <mergeCell ref="U18:W18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>